<commit_message>
update in sh expense
</commit_message>
<xml_diff>
--- a/sh expense.xlsx
+++ b/sh expense.xlsx
@@ -227,23 +227,11 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -255,6 +243,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,7 +552,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -569,246 +569,260 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="7"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="8"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="11">
+      <c r="A4" s="7">
         <v>245.7</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>614.20000000000005</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>999</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>10</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>4000</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="11">
+      <c r="A5" s="7">
         <v>326</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>913</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>1059</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>10</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="11">
+      <c r="A6" s="7">
         <v>221</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>1000</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="8"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="11">
+      <c r="A7" s="7">
         <v>360</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>274</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="8"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A8" s="12">
+      <c r="A8" s="8">
         <f>SUM(A4:A7)</f>
         <v>1152.7</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="9">
         <f>SUM(B4:B7)</f>
         <v>2801.2</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="9">
         <f>SUM(C4:C6)</f>
         <v>2058</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="9">
         <v>20</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="9">
         <v>4000</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="10">
         <f>SUM(A8:E8)</f>
         <v>10031.9</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1"/>
     <row r="11" spans="1:12">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-      <c r="I11" s="1" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="3"/>
+      <c r="I11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="7"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="8"/>
-      <c r="I12" s="2" t="s">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="4"/>
+      <c r="I12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A13" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <v>21019</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="1">
         <v>25000</v>
       </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2">
-        <v>46019</v>
+      <c r="K13" s="10">
+        <v>-3145</v>
+      </c>
+      <c r="L13" s="1">
+        <f>SUM(I13:K13)</f>
+        <v>42874</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="11">
+      <c r="A14" s="7">
         <v>80</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="8"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="11">
-        <v>2780</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="8"/>
+      <c r="A15" s="7">
+        <v>2705</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="11"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="8"/>
+      <c r="A16" s="7">
+        <v>320</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1">
+        <v>20</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="11"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="8"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A18" s="12">
+      <c r="A18" s="8">
         <f>SUM(A14:A17)</f>
-        <v>2860</v>
-      </c>
-      <c r="B18" s="13">
+        <v>3105</v>
+      </c>
+      <c r="B18" s="9">
         <f>SUM(B14:B17)</f>
         <v>0</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="9">
         <f>SUM(C14:C16)</f>
         <v>0</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="14">
+      <c r="D18" s="9">
+        <f>SUM(D16,D15,D14)</f>
+        <v>40</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10">
         <f>SUM(A18:E18)</f>
-        <v>2860</v>
+        <v>3145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>